<commit_message>
scheduling routing without conflicts
</commit_message>
<xml_diff>
--- a/Input data/Visibility_graph.xlsx
+++ b/Input data/Visibility_graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lichen/PycharmProjects/ACO_Example/Input data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740746B4-F22F-3446-83E6-203307D96D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E45AE7-09CB-9945-8510-D60C9901CF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2140" yWindow="2380" windowWidth="27680" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -387,431 +388,431 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EK141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="EH4" sqref="EH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:141">
-      <c r="A1" s="1">
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>6</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1">
         <v>9</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
         <v>10</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1">
         <v>11</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N1" s="1">
         <v>12</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="1">
         <v>13</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>14</v>
       </c>
-      <c r="P1" s="1">
+      <c r="Q1" s="1">
         <v>15</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="R1" s="1">
         <v>16</v>
       </c>
-      <c r="R1" s="1">
+      <c r="S1" s="1">
         <v>17</v>
       </c>
-      <c r="S1" s="1">
+      <c r="T1" s="1">
         <v>18</v>
       </c>
-      <c r="T1" s="1">
+      <c r="U1" s="1">
         <v>19</v>
       </c>
-      <c r="U1" s="1">
+      <c r="V1" s="1">
         <v>20</v>
       </c>
-      <c r="V1" s="1">
+      <c r="W1" s="1">
         <v>21</v>
       </c>
-      <c r="W1" s="1">
+      <c r="X1" s="1">
         <v>22</v>
       </c>
-      <c r="X1" s="1">
+      <c r="Y1" s="1">
         <v>23</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Z1" s="1">
         <v>24</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="AA1" s="1">
         <v>25</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AB1" s="1">
         <v>26</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AC1" s="1">
         <v>27</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AD1" s="1">
         <v>28</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AE1" s="1">
         <v>29</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AF1" s="1">
         <v>30</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AG1" s="1">
         <v>31</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="AH1" s="1">
         <v>32</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="AI1" s="1">
         <v>33</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AJ1" s="1">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AK1" s="1">
         <v>35</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AL1" s="1">
         <v>36</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AM1" s="1">
         <v>37</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AN1" s="1">
         <v>38</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AO1" s="1">
         <v>39</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AP1" s="1">
         <v>40</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AQ1" s="1">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AR1" s="1">
         <v>42</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AS1" s="1">
         <v>43</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AT1" s="1">
         <v>44</v>
       </c>
-      <c r="AT1" s="1">
+      <c r="AU1" s="1">
         <v>45</v>
       </c>
-      <c r="AU1" s="1">
+      <c r="AV1" s="1">
         <v>46</v>
       </c>
-      <c r="AV1" s="1">
+      <c r="AW1" s="1">
         <v>47</v>
       </c>
-      <c r="AW1" s="1">
+      <c r="AX1" s="1">
         <v>48</v>
       </c>
-      <c r="AX1" s="1">
+      <c r="AY1" s="1">
         <v>49</v>
       </c>
-      <c r="AY1" s="1">
+      <c r="AZ1" s="1">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1">
+      <c r="BA1" s="1">
         <v>51</v>
       </c>
-      <c r="BA1" s="1">
+      <c r="BB1" s="1">
         <v>52</v>
       </c>
-      <c r="BB1" s="1">
+      <c r="BC1" s="1">
         <v>53</v>
       </c>
-      <c r="BC1" s="1">
+      <c r="BD1" s="1">
         <v>54</v>
       </c>
-      <c r="BD1" s="1">
+      <c r="BE1" s="1">
         <v>55</v>
       </c>
-      <c r="BE1" s="1">
+      <c r="BF1" s="1">
         <v>56</v>
       </c>
-      <c r="BF1" s="1">
+      <c r="BG1" s="1">
         <v>57</v>
       </c>
-      <c r="BG1" s="1">
+      <c r="BH1" s="1">
         <v>58</v>
       </c>
-      <c r="BH1" s="1">
+      <c r="BI1" s="1">
         <v>59</v>
       </c>
-      <c r="BI1" s="1">
+      <c r="BJ1" s="1">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1">
+      <c r="BK1" s="1">
         <v>61</v>
       </c>
-      <c r="BK1" s="1">
+      <c r="BL1" s="1">
         <v>62</v>
       </c>
-      <c r="BL1" s="1">
+      <c r="BM1" s="1">
         <v>63</v>
       </c>
-      <c r="BM1" s="1">
+      <c r="BN1" s="1">
         <v>64</v>
       </c>
-      <c r="BN1" s="1">
+      <c r="BO1" s="1">
         <v>65</v>
       </c>
-      <c r="BO1" s="1">
+      <c r="BP1" s="1">
         <v>66</v>
       </c>
-      <c r="BP1" s="1">
+      <c r="BQ1" s="1">
         <v>67</v>
       </c>
-      <c r="BQ1" s="1">
+      <c r="BR1" s="1">
         <v>68</v>
       </c>
-      <c r="BR1" s="1">
+      <c r="BS1" s="1">
         <v>69</v>
       </c>
-      <c r="BS1" s="1">
+      <c r="BT1" s="1">
         <v>70</v>
       </c>
-      <c r="BT1" s="1">
+      <c r="BU1" s="1">
         <v>71</v>
       </c>
-      <c r="BU1" s="1">
+      <c r="BV1" s="1">
         <v>72</v>
       </c>
-      <c r="BV1" s="1">
+      <c r="BW1" s="1">
         <v>73</v>
       </c>
-      <c r="BW1" s="1">
+      <c r="BX1" s="1">
         <v>74</v>
       </c>
-      <c r="BX1" s="1">
+      <c r="BY1" s="1">
         <v>75</v>
       </c>
-      <c r="BY1" s="1">
+      <c r="BZ1" s="1">
         <v>76</v>
       </c>
-      <c r="BZ1" s="1">
+      <c r="CA1" s="1">
         <v>77</v>
       </c>
-      <c r="CA1" s="1">
+      <c r="CB1" s="1">
         <v>78</v>
       </c>
-      <c r="CB1" s="1">
+      <c r="CC1" s="1">
         <v>79</v>
       </c>
-      <c r="CC1" s="1">
+      <c r="CD1" s="1">
         <v>80</v>
       </c>
-      <c r="CD1" s="1">
+      <c r="CE1" s="1">
         <v>81</v>
       </c>
-      <c r="CE1" s="1">
+      <c r="CF1" s="1">
         <v>82</v>
       </c>
-      <c r="CF1" s="1">
+      <c r="CG1" s="1">
         <v>83</v>
       </c>
-      <c r="CG1" s="1">
+      <c r="CH1" s="1">
         <v>84</v>
       </c>
-      <c r="CH1" s="1">
+      <c r="CI1" s="1">
         <v>85</v>
       </c>
-      <c r="CI1" s="1">
+      <c r="CJ1" s="1">
         <v>86</v>
       </c>
-      <c r="CJ1" s="1">
+      <c r="CK1" s="1">
         <v>87</v>
       </c>
-      <c r="CK1" s="1">
+      <c r="CL1" s="1">
         <v>88</v>
       </c>
-      <c r="CL1" s="1">
+      <c r="CM1" s="1">
         <v>89</v>
       </c>
-      <c r="CM1" s="1">
+      <c r="CN1" s="1">
         <v>90</v>
       </c>
-      <c r="CN1" s="1">
+      <c r="CO1" s="1">
         <v>91</v>
       </c>
-      <c r="CO1" s="1">
+      <c r="CP1" s="1">
         <v>92</v>
       </c>
-      <c r="CP1" s="1">
+      <c r="CQ1" s="1">
         <v>93</v>
       </c>
-      <c r="CQ1" s="1">
+      <c r="CR1" s="1">
         <v>94</v>
       </c>
-      <c r="CR1" s="1">
+      <c r="CS1" s="1">
         <v>95</v>
       </c>
-      <c r="CS1" s="1">
+      <c r="CT1" s="1">
         <v>96</v>
       </c>
-      <c r="CT1" s="1">
+      <c r="CU1" s="1">
         <v>97</v>
       </c>
-      <c r="CU1" s="1">
+      <c r="CV1" s="1">
         <v>98</v>
       </c>
-      <c r="CV1" s="1">
+      <c r="CW1" s="1">
         <v>99</v>
       </c>
-      <c r="CW1" s="1">
+      <c r="CX1" s="1">
         <v>100</v>
       </c>
-      <c r="CX1" s="1">
+      <c r="CY1" s="1">
         <v>101</v>
       </c>
-      <c r="CY1" s="1">
+      <c r="CZ1" s="1">
         <v>102</v>
       </c>
-      <c r="CZ1" s="1">
+      <c r="DA1" s="1">
         <v>103</v>
       </c>
-      <c r="DA1" s="1">
+      <c r="DB1" s="1">
         <v>104</v>
       </c>
-      <c r="DB1" s="1">
+      <c r="DC1" s="1">
         <v>105</v>
       </c>
-      <c r="DC1" s="1">
+      <c r="DD1" s="1">
         <v>106</v>
       </c>
-      <c r="DD1" s="1">
+      <c r="DE1" s="1">
         <v>107</v>
       </c>
-      <c r="DE1" s="1">
+      <c r="DF1" s="1">
         <v>108</v>
       </c>
-      <c r="DF1" s="1">
+      <c r="DG1" s="1">
         <v>109</v>
       </c>
-      <c r="DG1" s="1">
+      <c r="DH1" s="1">
         <v>110</v>
       </c>
-      <c r="DH1" s="1">
+      <c r="DI1" s="1">
         <v>111</v>
       </c>
-      <c r="DI1" s="1">
+      <c r="DJ1" s="1">
         <v>112</v>
       </c>
-      <c r="DJ1" s="1">
+      <c r="DK1" s="1">
         <v>113</v>
       </c>
-      <c r="DK1" s="1">
+      <c r="DL1" s="1">
         <v>114</v>
       </c>
-      <c r="DL1" s="1">
+      <c r="DM1" s="1">
         <v>115</v>
       </c>
-      <c r="DM1" s="1">
+      <c r="DN1" s="1">
         <v>116</v>
       </c>
-      <c r="DN1" s="1">
+      <c r="DO1" s="1">
         <v>117</v>
       </c>
-      <c r="DO1" s="1">
+      <c r="DP1" s="1">
         <v>118</v>
       </c>
-      <c r="DP1" s="1">
+      <c r="DQ1" s="1">
         <v>119</v>
       </c>
-      <c r="DQ1" s="1">
+      <c r="DR1" s="1">
         <v>120</v>
       </c>
-      <c r="DR1" s="1">
+      <c r="DS1" s="1">
         <v>121</v>
       </c>
-      <c r="DS1" s="1">
+      <c r="DT1" s="1">
         <v>122</v>
       </c>
-      <c r="DT1" s="1">
+      <c r="DU1" s="1">
         <v>123</v>
       </c>
-      <c r="DU1" s="1">
+      <c r="DV1" s="1">
         <v>124</v>
       </c>
-      <c r="DV1" s="1">
+      <c r="DW1" s="1">
         <v>125</v>
       </c>
-      <c r="DW1" s="1">
+      <c r="DX1" s="1">
         <v>126</v>
       </c>
-      <c r="DX1" s="1">
+      <c r="DY1" s="1">
         <v>127</v>
       </c>
-      <c r="DY1" s="1">
+      <c r="DZ1" s="1">
         <v>128</v>
       </c>
-      <c r="DZ1" s="1">
+      <c r="EA1" s="1">
         <v>129</v>
       </c>
-      <c r="EA1" s="1">
+      <c r="EB1" s="1">
         <v>130</v>
       </c>
-      <c r="EB1" s="1">
+      <c r="EC1" s="1">
         <v>131</v>
       </c>
-      <c r="EC1" s="1">
+      <c r="ED1" s="1">
         <v>132</v>
       </c>
-      <c r="ED1" s="1">
+      <c r="EE1" s="1">
         <v>133</v>
       </c>
-      <c r="EE1" s="1">
+      <c r="EF1" s="1">
         <v>134</v>
       </c>
-      <c r="EF1" s="1">
+      <c r="EG1" s="1">
         <v>135</v>
       </c>
-      <c r="EG1" s="1">
-        <v>136</v>
-      </c>
       <c r="EH1" s="1">
+        <v>136</v>
+      </c>
+      <c r="EI1" s="1">
         <v>137</v>
       </c>
-      <c r="EI1" s="1">
+      <c r="EJ1" s="1">
         <v>138</v>
       </c>
-      <c r="EJ1" s="1">
+      <c r="EK1" s="1">
         <v>139</v>
       </c>
     </row>

</xml_diff>